<commit_message>
Atualização semiautomática dos dados - 31/8/2021
</commit_message>
<xml_diff>
--- a/dadosIsolamento.xlsx
+++ b/dadosIsolamento.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="546">
   <si>
     <t>Data</t>
   </si>
@@ -1625,6 +1625,12 @@
   </si>
   <si>
     <t>08/28/2021</t>
+  </si>
+  <si>
+    <t>08/29/2021</t>
+  </si>
+  <si>
+    <t>08/30/2021</t>
   </si>
   <si>
     <t>Quinta-Feira</t>
@@ -2003,7 +2009,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D534"/>
+  <dimension ref="A1:D536"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2034,7 +2040,7 @@
         <v>0.4</v>
       </c>
       <c r="D2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2048,7 +2054,7 @@
         <v>0.38</v>
       </c>
       <c r="D3" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2062,7 +2068,7 @@
         <v>0.35</v>
       </c>
       <c r="D4" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2076,7 +2082,7 @@
         <v>0.37</v>
       </c>
       <c r="D5" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2090,7 +2096,7 @@
         <v>0.43</v>
       </c>
       <c r="D6" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2104,7 +2110,7 @@
         <v>0.42</v>
       </c>
       <c r="D7" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2118,7 +2124,7 @@
         <v>0.44</v>
       </c>
       <c r="D8" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2132,7 +2138,7 @@
         <v>0.46</v>
       </c>
       <c r="D9" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2146,7 +2152,7 @@
         <v>0.58</v>
       </c>
       <c r="D10" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2160,7 +2166,7 @@
         <v>0.57</v>
       </c>
       <c r="D11" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2174,7 +2180,7 @@
         <v>0.53</v>
       </c>
       <c r="D12" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2188,7 +2194,7 @@
         <v>0.55</v>
       </c>
       <c r="D13" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2202,7 +2208,7 @@
         <v>0.55</v>
       </c>
       <c r="D14" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2216,7 +2222,7 @@
         <v>0.54</v>
       </c>
       <c r="D15" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2230,7 +2236,7 @@
         <v>0.54</v>
       </c>
       <c r="D16" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2244,7 +2250,7 @@
         <v>0.57</v>
       </c>
       <c r="D17" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2258,7 +2264,7 @@
         <v>0.59</v>
       </c>
       <c r="D18" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2272,7 +2278,7 @@
         <v>0.57</v>
       </c>
       <c r="D19" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2286,7 +2292,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="D20" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2300,7 +2306,7 @@
         <v>0.55</v>
       </c>
       <c r="D21" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2314,7 +2320,7 @@
         <v>0.55</v>
       </c>
       <c r="D22" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2328,7 +2334,7 @@
         <v>0.55</v>
       </c>
       <c r="D23" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2342,7 +2348,7 @@
         <v>0.58</v>
       </c>
       <c r="D24" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2356,7 +2362,7 @@
         <v>0.58</v>
       </c>
       <c r="D25" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2370,7 +2376,7 @@
         <v>0.53</v>
       </c>
       <c r="D26" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2384,7 +2390,7 @@
         <v>0.51</v>
       </c>
       <c r="D27" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2398,7 +2404,7 @@
         <v>0.48</v>
       </c>
       <c r="D28" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2412,7 +2418,7 @@
         <v>0.5</v>
       </c>
       <c r="D29" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2426,7 +2432,7 @@
         <v>0.61</v>
       </c>
       <c r="D30" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2440,7 +2446,7 @@
         <v>0.54</v>
       </c>
       <c r="D31" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2454,7 +2460,7 @@
         <v>0.57</v>
       </c>
       <c r="D32" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2468,7 +2474,7 @@
         <v>0.49</v>
       </c>
       <c r="D33" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2482,7 +2488,7 @@
         <v>0.5</v>
       </c>
       <c r="D34" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2496,7 +2502,7 @@
         <v>0.5</v>
       </c>
       <c r="D35" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2510,7 +2516,7 @@
         <v>0.49</v>
       </c>
       <c r="D36" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2524,7 +2530,7 @@
         <v>0.48</v>
       </c>
       <c r="D37" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2538,7 +2544,7 @@
         <v>0.53</v>
       </c>
       <c r="D38" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2552,7 +2558,7 @@
         <v>0.58</v>
       </c>
       <c r="D39" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2566,7 +2572,7 @@
         <v>0.49</v>
       </c>
       <c r="D40" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2580,7 +2586,7 @@
         <v>0.57</v>
       </c>
       <c r="D41" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2594,7 +2600,7 @@
         <v>0.47</v>
       </c>
       <c r="D42" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2608,7 +2614,7 @@
         <v>0.46</v>
       </c>
       <c r="D43" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2622,7 +2628,7 @@
         <v>0.47</v>
       </c>
       <c r="D44" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2636,7 +2642,7 @@
         <v>0.52</v>
       </c>
       <c r="D45" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2650,7 +2656,7 @@
         <v>0.57</v>
       </c>
       <c r="D46" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2664,7 +2670,7 @@
         <v>0.47</v>
       </c>
       <c r="D47" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2678,7 +2684,7 @@
         <v>0.46</v>
       </c>
       <c r="D48" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2692,7 +2698,7 @@
         <v>0.47</v>
       </c>
       <c r="D49" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2706,7 +2712,7 @@
         <v>0.46</v>
       </c>
       <c r="D50" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2720,7 +2726,7 @@
         <v>0.53</v>
       </c>
       <c r="D51" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2734,7 +2740,7 @@
         <v>0.5</v>
       </c>
       <c r="D52" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2748,7 +2754,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="D53" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2762,7 +2768,7 @@
         <v>0.46</v>
       </c>
       <c r="D54" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2776,7 +2782,7 @@
         <v>0.46</v>
       </c>
       <c r="D55" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2790,7 +2796,7 @@
         <v>0.45</v>
       </c>
       <c r="D56" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2804,7 +2810,7 @@
         <v>0.45</v>
       </c>
       <c r="D57" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2818,7 +2824,7 @@
         <v>0.44</v>
       </c>
       <c r="D58" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2832,7 +2838,7 @@
         <v>0.47</v>
       </c>
       <c r="D59" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2846,7 +2852,7 @@
         <v>0.51</v>
       </c>
       <c r="D60" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2860,7 +2866,7 @@
         <v>0.46</v>
       </c>
       <c r="D61" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2874,7 +2880,7 @@
         <v>0.46</v>
       </c>
       <c r="D62" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2888,7 +2894,7 @@
         <v>0.45</v>
       </c>
       <c r="D63" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2902,7 +2908,7 @@
         <v>0.46</v>
       </c>
       <c r="D64" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2916,7 +2922,7 @@
         <v>0.45</v>
       </c>
       <c r="D65" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2930,7 +2936,7 @@
         <v>0.47</v>
       </c>
       <c r="D66" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2944,7 +2950,7 @@
         <v>0.51</v>
       </c>
       <c r="D67" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2958,7 +2964,7 @@
         <v>0.45</v>
       </c>
       <c r="D68" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2972,7 +2978,7 @@
         <v>0.45</v>
       </c>
       <c r="D69" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2986,7 +2992,7 @@
         <v>0.44</v>
       </c>
       <c r="D70" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -3000,7 +3006,7 @@
         <v>0.45</v>
       </c>
       <c r="D71" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -3014,7 +3020,7 @@
         <v>0.44</v>
       </c>
       <c r="D72" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -3028,7 +3034,7 @@
         <v>0.47</v>
       </c>
       <c r="D73" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -3042,7 +3048,7 @@
         <v>0.53</v>
       </c>
       <c r="D74" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -3056,7 +3062,7 @@
         <v>0.5</v>
       </c>
       <c r="D75" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -3070,7 +3076,7 @@
         <v>0.44</v>
       </c>
       <c r="D76" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -3084,7 +3090,7 @@
         <v>0.44</v>
       </c>
       <c r="D77" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -3098,7 +3104,7 @@
         <v>0.44</v>
       </c>
       <c r="D78" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -3112,7 +3118,7 @@
         <v>0.44</v>
       </c>
       <c r="D79" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -3126,7 +3132,7 @@
         <v>0.47</v>
       </c>
       <c r="D80" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -3140,7 +3146,7 @@
         <v>0.5</v>
       </c>
       <c r="D81" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3154,7 +3160,7 @@
         <v>0.44</v>
       </c>
       <c r="D82" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -3168,7 +3174,7 @@
         <v>0.44</v>
       </c>
       <c r="D83" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -3182,7 +3188,7 @@
         <v>0.43</v>
       </c>
       <c r="D84" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3196,7 +3202,7 @@
         <v>0.44</v>
       </c>
       <c r="D85" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3210,7 +3216,7 @@
         <v>0.42</v>
       </c>
       <c r="D86" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3224,7 +3230,7 @@
         <v>0.45</v>
       </c>
       <c r="D87" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3238,7 +3244,7 @@
         <v>0.49</v>
       </c>
       <c r="D88" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3252,7 +3258,7 @@
         <v>0.44</v>
       </c>
       <c r="D89" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3266,7 +3272,7 @@
         <v>0.43</v>
       </c>
       <c r="D90" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3280,7 +3286,7 @@
         <v>0.4</v>
       </c>
       <c r="D91" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3294,7 +3300,7 @@
         <v>0.45</v>
       </c>
       <c r="D92" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3308,7 +3314,7 @@
         <v>0.41</v>
       </c>
       <c r="D93" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3322,7 +3328,7 @@
         <v>0.43</v>
       </c>
       <c r="D94" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3336,7 +3342,7 @@
         <v>0.47</v>
       </c>
       <c r="D95" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3350,7 +3356,7 @@
         <v>0.42</v>
       </c>
       <c r="D96" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3364,7 +3370,7 @@
         <v>0.42</v>
       </c>
       <c r="D97" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3378,7 +3384,7 @@
         <v>0.42</v>
       </c>
       <c r="D98" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3392,7 +3398,7 @@
         <v>0.41</v>
       </c>
       <c r="D99" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3406,7 +3412,7 @@
         <v>0.4</v>
       </c>
       <c r="D100" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3420,7 +3426,7 @@
         <v>0.44</v>
       </c>
       <c r="D101" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3434,7 +3440,7 @@
         <v>0.48</v>
       </c>
       <c r="D102" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3448,7 +3454,7 @@
         <v>0.42</v>
       </c>
       <c r="D103" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3462,7 +3468,7 @@
         <v>0.42</v>
       </c>
       <c r="D104" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3476,7 +3482,7 @@
         <v>0.43</v>
       </c>
       <c r="D105" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3490,7 +3496,7 @@
         <v>0.43</v>
       </c>
       <c r="D106" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3504,7 +3510,7 @@
         <v>0.42</v>
       </c>
       <c r="D107" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3518,7 +3524,7 @@
         <v>0.44</v>
       </c>
       <c r="D108" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3532,7 +3538,7 @@
         <v>0.49</v>
       </c>
       <c r="D109" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3546,7 +3552,7 @@
         <v>0.46</v>
       </c>
       <c r="D110" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3560,7 +3566,7 @@
         <v>0.43</v>
       </c>
       <c r="D111" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3574,7 +3580,7 @@
         <v>0.42</v>
       </c>
       <c r="D112" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3588,7 +3594,7 @@
         <v>0.42</v>
       </c>
       <c r="D113" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3602,7 +3608,7 @@
         <v>0.41</v>
       </c>
       <c r="D114" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3616,7 +3622,7 @@
         <v>0.44</v>
       </c>
       <c r="D115" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3630,7 +3636,7 @@
         <v>0.48</v>
       </c>
       <c r="D116" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3644,7 +3650,7 @@
         <v>0.42</v>
       </c>
       <c r="D117" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3658,7 +3664,7 @@
         <v>0.42</v>
       </c>
       <c r="D118" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3672,7 +3678,7 @@
         <v>0.42</v>
       </c>
       <c r="D119" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3686,7 +3692,7 @@
         <v>0.42</v>
       </c>
       <c r="D120" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3700,7 +3706,7 @@
         <v>0.4</v>
       </c>
       <c r="D121" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3714,7 +3720,7 @@
         <v>0.44</v>
       </c>
       <c r="D122" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3728,7 +3734,7 @@
         <v>0.48</v>
       </c>
       <c r="D123" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3742,7 +3748,7 @@
         <v>0.42</v>
       </c>
       <c r="D124" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3756,7 +3762,7 @@
         <v>0.42</v>
       </c>
       <c r="D125" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3770,7 +3776,7 @@
         <v>0.41</v>
       </c>
       <c r="D126" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3784,7 +3790,7 @@
         <v>0.42</v>
       </c>
       <c r="D127" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3798,7 +3804,7 @@
         <v>0.42</v>
       </c>
       <c r="D128" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3812,7 +3818,7 @@
         <v>0.44</v>
       </c>
       <c r="D129" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3826,7 +3832,7 @@
         <v>0.49</v>
       </c>
       <c r="D130" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3840,7 +3846,7 @@
         <v>0.42</v>
       </c>
       <c r="D131" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3854,7 +3860,7 @@
         <v>0.41</v>
       </c>
       <c r="D132" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3868,7 +3874,7 @@
         <v>0.4</v>
       </c>
       <c r="D133" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3882,7 +3888,7 @@
         <v>0.4</v>
       </c>
       <c r="D134" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3896,7 +3902,7 @@
         <v>0.39</v>
       </c>
       <c r="D135" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3910,7 +3916,7 @@
         <v>0.44</v>
       </c>
       <c r="D136" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3924,7 +3930,7 @@
         <v>0.49</v>
       </c>
       <c r="D137" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3938,7 +3944,7 @@
         <v>0.41</v>
       </c>
       <c r="D138" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3952,7 +3958,7 @@
         <v>0.41</v>
       </c>
       <c r="D139" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3966,7 +3972,7 @@
         <v>0.41</v>
       </c>
       <c r="D140" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3980,7 +3986,7 @@
         <v>0.41</v>
       </c>
       <c r="D141" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3994,7 +4000,7 @@
         <v>0.41</v>
       </c>
       <c r="D142" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -4008,7 +4014,7 @@
         <v>0.41</v>
       </c>
       <c r="D143" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -4022,7 +4028,7 @@
         <v>0.48</v>
       </c>
       <c r="D144" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -4036,7 +4042,7 @@
         <v>0.4</v>
       </c>
       <c r="D145" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -4050,7 +4056,7 @@
         <v>0.4</v>
       </c>
       <c r="D146" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -4064,7 +4070,7 @@
         <v>0.39</v>
       </c>
       <c r="D147" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -4078,7 +4084,7 @@
         <v>0.31</v>
       </c>
       <c r="D148" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -4092,7 +4098,7 @@
         <v>0.38</v>
       </c>
       <c r="D149" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -4106,7 +4112,7 @@
         <v>0.41</v>
       </c>
       <c r="D150" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -4120,7 +4126,7 @@
         <v>0.46</v>
       </c>
       <c r="D151" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -4134,7 +4140,7 @@
         <v>0.41</v>
       </c>
       <c r="D152" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -4148,7 +4154,7 @@
         <v>0.4</v>
       </c>
       <c r="D153" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -4162,7 +4168,7 @@
         <v>0.4</v>
       </c>
       <c r="D154" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -4176,7 +4182,7 @@
         <v>0.39</v>
       </c>
       <c r="D155" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -4190,7 +4196,7 @@
         <v>0.41</v>
       </c>
       <c r="D156" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -4204,7 +4210,7 @@
         <v>0.42</v>
       </c>
       <c r="D157" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -4218,7 +4224,7 @@
         <v>0.49</v>
       </c>
       <c r="D158" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4232,7 +4238,7 @@
         <v>0.41</v>
       </c>
       <c r="D159" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4246,7 +4252,7 @@
         <v>0.4</v>
       </c>
       <c r="D160" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4260,7 +4266,7 @@
         <v>0.41</v>
       </c>
       <c r="D161" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4274,7 +4280,7 @@
         <v>0.4</v>
       </c>
       <c r="D162" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4288,7 +4294,7 @@
         <v>0.4</v>
       </c>
       <c r="D163" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4302,7 +4308,7 @@
         <v>0.42</v>
       </c>
       <c r="D164" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4316,7 +4322,7 @@
         <v>0.48</v>
       </c>
       <c r="D165" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4330,7 +4336,7 @@
         <v>0.4</v>
       </c>
       <c r="D166" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4344,7 +4350,7 @@
         <v>0.4</v>
       </c>
       <c r="D167" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4358,7 +4364,7 @@
         <v>0.4</v>
       </c>
       <c r="D168" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4372,7 +4378,7 @@
         <v>0.4</v>
       </c>
       <c r="D169" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4386,7 +4392,7 @@
         <v>0.39</v>
       </c>
       <c r="D170" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4400,7 +4406,7 @@
         <v>0.4</v>
       </c>
       <c r="D171" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4414,7 +4420,7 @@
         <v>0.46</v>
       </c>
       <c r="D172" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4428,7 +4434,7 @@
         <v>0.39</v>
       </c>
       <c r="D173" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4442,7 +4448,7 @@
         <v>0.4</v>
       </c>
       <c r="D174" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4456,7 +4462,7 @@
         <v>0.4</v>
       </c>
       <c r="D175" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4470,7 +4476,7 @@
         <v>0.39</v>
       </c>
       <c r="D176" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4484,7 +4490,7 @@
         <v>0.35</v>
       </c>
       <c r="D177" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4498,7 +4504,7 @@
         <v>0.4</v>
       </c>
       <c r="D178" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4512,7 +4518,7 @@
         <v>0.44</v>
       </c>
       <c r="D179" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4526,7 +4532,7 @@
         <v>0.46</v>
       </c>
       <c r="D180" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4540,7 +4546,7 @@
         <v>0.38</v>
       </c>
       <c r="D181" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4554,7 +4560,7 @@
         <v>0.39</v>
       </c>
       <c r="D182" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4568,7 +4574,7 @@
         <v>0.39</v>
       </c>
       <c r="D183" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4582,7 +4588,7 @@
         <v>0.39</v>
       </c>
       <c r="D184" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4596,7 +4602,7 @@
         <v>0.41</v>
       </c>
       <c r="D185" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4610,7 +4616,7 @@
         <v>0.45</v>
       </c>
       <c r="D186" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4624,7 +4630,7 @@
         <v>0.39</v>
       </c>
       <c r="D187" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4638,7 +4644,7 @@
         <v>0.4</v>
       </c>
       <c r="D188" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4652,7 +4658,7 @@
         <v>0.4</v>
       </c>
       <c r="D189" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4666,7 +4672,7 @@
         <v>0.4</v>
       </c>
       <c r="D190" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4680,7 +4686,7 @@
         <v>0.39</v>
       </c>
       <c r="D191" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4694,7 +4700,7 @@
         <v>0.4</v>
       </c>
       <c r="D192" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4708,7 +4714,7 @@
         <v>0.47</v>
       </c>
       <c r="D193" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4722,7 +4728,7 @@
         <v>0.4</v>
       </c>
       <c r="D194" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4736,7 +4742,7 @@
         <v>0.41</v>
       </c>
       <c r="D195" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4750,7 +4756,7 @@
         <v>0.4</v>
       </c>
       <c r="D196" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4764,7 +4770,7 @@
         <v>0.4</v>
       </c>
       <c r="D197" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4778,7 +4784,7 @@
         <v>0.39</v>
       </c>
       <c r="D198" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4792,7 +4798,7 @@
         <v>0.41</v>
       </c>
       <c r="D199" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4806,7 +4812,7 @@
         <v>0.45</v>
       </c>
       <c r="D200" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4820,7 +4826,7 @@
         <v>0.41</v>
       </c>
       <c r="D201" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -4834,7 +4840,7 @@
         <v>0.38</v>
       </c>
       <c r="D202" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -4848,7 +4854,7 @@
         <v>0.38</v>
       </c>
       <c r="D203" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4862,7 +4868,7 @@
         <v>0.4</v>
       </c>
       <c r="D204" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4876,7 +4882,7 @@
         <v>0.39</v>
       </c>
       <c r="D205" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4890,7 +4896,7 @@
         <v>0.4</v>
       </c>
       <c r="D206" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4904,7 +4910,7 @@
         <v>0.45</v>
       </c>
       <c r="D207" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4918,7 +4924,7 @@
         <v>0.39</v>
       </c>
       <c r="D208" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4932,7 +4938,7 @@
         <v>0.38</v>
       </c>
       <c r="D209" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4946,7 +4952,7 @@
         <v>0.39</v>
       </c>
       <c r="D210" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4960,7 +4966,7 @@
         <v>0.4</v>
       </c>
       <c r="D211" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4974,7 +4980,7 @@
         <v>0.39</v>
       </c>
       <c r="D212" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4988,7 +4994,7 @@
         <v>0.39</v>
       </c>
       <c r="D213" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -5002,7 +5008,7 @@
         <v>0.44</v>
       </c>
       <c r="D214" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -5016,7 +5022,7 @@
         <v>0.47</v>
       </c>
       <c r="D215" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -5030,7 +5036,7 @@
         <v>0.38</v>
       </c>
       <c r="D216" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -5044,7 +5050,7 @@
         <v>0.39</v>
       </c>
       <c r="D217" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -5058,7 +5064,7 @@
         <v>0.39</v>
       </c>
       <c r="D218" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -5072,7 +5078,7 @@
         <v>0.4</v>
       </c>
       <c r="D219" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -5086,7 +5092,7 @@
         <v>0.41</v>
       </c>
       <c r="D220" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -5100,7 +5106,7 @@
         <v>0.46</v>
       </c>
       <c r="D221" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -5114,7 +5120,7 @@
         <v>0.39</v>
       </c>
       <c r="D222" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -5128,7 +5134,7 @@
         <v>0.39</v>
       </c>
       <c r="D223" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -5142,7 +5148,7 @@
         <v>0.39</v>
       </c>
       <c r="D224" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5156,7 +5162,7 @@
         <v>0.4</v>
       </c>
       <c r="D225" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5170,7 +5176,7 @@
         <v>0.38</v>
       </c>
       <c r="D226" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -5184,7 +5190,7 @@
         <v>0.41</v>
       </c>
       <c r="D227" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5198,7 +5204,7 @@
         <v>0.46</v>
       </c>
       <c r="D228" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5212,7 +5218,7 @@
         <v>0.39</v>
       </c>
       <c r="D229" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5226,7 +5232,7 @@
         <v>0.4</v>
       </c>
       <c r="D230" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5240,7 +5246,7 @@
         <v>0.4</v>
       </c>
       <c r="D231" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5254,7 +5260,7 @@
         <v>0.39</v>
       </c>
       <c r="D232" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5268,7 +5274,7 @@
         <v>0.38</v>
       </c>
       <c r="D233" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5282,7 +5288,7 @@
         <v>0.41</v>
       </c>
       <c r="D234" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5296,7 +5302,7 @@
         <v>0.46</v>
       </c>
       <c r="D235" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5310,7 +5316,7 @@
         <v>0.46</v>
       </c>
       <c r="D236" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5324,7 +5330,7 @@
         <v>0.39</v>
       </c>
       <c r="D237" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5338,7 +5344,7 @@
         <v>0.4</v>
       </c>
       <c r="D238" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5352,7 +5358,7 @@
         <v>0.38</v>
       </c>
       <c r="D239" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5366,7 +5372,7 @@
         <v>0.38</v>
       </c>
       <c r="D240" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5380,7 +5386,7 @@
         <v>0.41</v>
       </c>
       <c r="D241" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5394,7 +5400,7 @@
         <v>0.44</v>
       </c>
       <c r="D242" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5408,7 +5414,7 @@
         <v>0.39</v>
       </c>
       <c r="D243" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5422,7 +5428,7 @@
         <v>0.38</v>
       </c>
       <c r="D244" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5436,7 +5442,7 @@
         <v>0.4</v>
       </c>
       <c r="D245" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5450,7 +5456,7 @@
         <v>0.38</v>
       </c>
       <c r="D246" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5464,7 +5470,7 @@
         <v>0.38</v>
       </c>
       <c r="D247" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5478,7 +5484,7 @@
         <v>0.41</v>
       </c>
       <c r="D248" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5492,7 +5498,7 @@
         <v>0.44</v>
       </c>
       <c r="D249" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5506,7 +5512,7 @@
         <v>0.38</v>
       </c>
       <c r="D250" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5520,7 +5526,7 @@
         <v>0.38</v>
       </c>
       <c r="D251" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5534,7 +5540,7 @@
         <v>0.39</v>
       </c>
       <c r="D252" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5548,7 +5554,7 @@
         <v>0.38</v>
       </c>
       <c r="D253" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5562,7 +5568,7 @@
         <v>0.4</v>
       </c>
       <c r="D254" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5576,7 +5582,7 @@
         <v>0.41</v>
       </c>
       <c r="D255" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -5590,7 +5596,7 @@
         <v>0.43</v>
       </c>
       <c r="D256" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5604,7 +5610,7 @@
         <v>0.39</v>
       </c>
       <c r="D257" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -5618,7 +5624,7 @@
         <v>0.39</v>
       </c>
       <c r="D258" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5632,7 +5638,7 @@
         <v>0.38</v>
       </c>
       <c r="D259" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -5646,7 +5652,7 @@
         <v>0.39</v>
       </c>
       <c r="D260" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -5660,7 +5666,7 @@
         <v>0.4</v>
       </c>
       <c r="D261" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -5674,7 +5680,7 @@
         <v>0.41</v>
       </c>
       <c r="D262" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -5688,7 +5694,7 @@
         <v>0.45</v>
       </c>
       <c r="D263" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5702,7 +5708,7 @@
         <v>0.39</v>
       </c>
       <c r="D264" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -5716,7 +5722,7 @@
         <v>0.38</v>
       </c>
       <c r="D265" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -5730,7 +5736,7 @@
         <v>0.39</v>
       </c>
       <c r="D266" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -5744,7 +5750,7 @@
         <v>0.39</v>
       </c>
       <c r="D267" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -5758,7 +5764,7 @@
         <v>0.38</v>
       </c>
       <c r="D268" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -5772,7 +5778,7 @@
         <v>0.39</v>
       </c>
       <c r="D269" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5786,7 +5792,7 @@
         <v>0.43</v>
       </c>
       <c r="D270" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -5800,7 +5806,7 @@
         <v>0.39</v>
       </c>
       <c r="D271" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -5814,7 +5820,7 @@
         <v>0.42</v>
       </c>
       <c r="D272" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5828,7 +5834,7 @@
         <v>0.38</v>
       </c>
       <c r="D273" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -5842,7 +5848,7 @@
         <v>0.39</v>
       </c>
       <c r="D274" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -5856,7 +5862,7 @@
         <v>0.38</v>
       </c>
       <c r="D275" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -5870,7 +5876,7 @@
         <v>0.4</v>
       </c>
       <c r="D276" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5884,7 +5890,7 @@
         <v>0.43</v>
       </c>
       <c r="D277" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -5898,7 +5904,7 @@
         <v>0.4</v>
       </c>
       <c r="D278" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5912,7 +5918,7 @@
         <v>0.41</v>
       </c>
       <c r="D279" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5926,7 +5932,7 @@
         <v>0.39</v>
       </c>
       <c r="D280" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5940,7 +5946,7 @@
         <v>0.4</v>
       </c>
       <c r="D281" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5954,7 +5960,7 @@
         <v>0.38</v>
       </c>
       <c r="D282" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5968,7 +5974,7 @@
         <v>0.4</v>
       </c>
       <c r="D283" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5982,7 +5988,7 @@
         <v>0.44</v>
       </c>
       <c r="D284" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5996,7 +6002,7 @@
         <v>0.39</v>
       </c>
       <c r="D285" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -6010,7 +6016,7 @@
         <v>0.4</v>
       </c>
       <c r="D286" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -6024,7 +6030,7 @@
         <v>0.38</v>
       </c>
       <c r="D287" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -6038,7 +6044,7 @@
         <v>0.4</v>
       </c>
       <c r="D288" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -6052,7 +6058,7 @@
         <v>0.48</v>
       </c>
       <c r="D289" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -6066,7 +6072,7 @@
         <v>0.46</v>
       </c>
       <c r="D290" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -6080,7 +6086,7 @@
         <v>0.5</v>
       </c>
       <c r="D291" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -6094,7 +6100,7 @@
         <v>0.41</v>
       </c>
       <c r="D292" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -6108,7 +6114,7 @@
         <v>0.37</v>
       </c>
       <c r="D293" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -6122,7 +6128,7 @@
         <v>0.39</v>
       </c>
       <c r="D294" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -6136,7 +6142,7 @@
         <v>0.41</v>
       </c>
       <c r="D295" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -6150,7 +6156,7 @@
         <v>0.48</v>
       </c>
       <c r="D296" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -6164,7 +6170,7 @@
         <v>0.47</v>
       </c>
       <c r="D297" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -6178,7 +6184,7 @@
         <v>0.48</v>
       </c>
       <c r="D298" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -6192,7 +6198,7 @@
         <v>0.36</v>
       </c>
       <c r="D299" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -6206,7 +6212,7 @@
         <v>0.39</v>
       </c>
       <c r="D300" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -6220,7 +6226,7 @@
         <v>0.47</v>
       </c>
       <c r="D301" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -6234,7 +6240,7 @@
         <v>0.4</v>
       </c>
       <c r="D302" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -6248,7 +6254,7 @@
         <v>0.39</v>
       </c>
       <c r="D303" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -6262,7 +6268,7 @@
         <v>0.46</v>
       </c>
       <c r="D304" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -6276,7 +6282,7 @@
         <v>0.46</v>
       </c>
       <c r="D305" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -6290,7 +6296,7 @@
         <v>0.4</v>
       </c>
       <c r="D306" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6304,7 +6310,7 @@
         <v>0.4</v>
       </c>
       <c r="D307" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -6318,7 +6324,7 @@
         <v>0.4</v>
       </c>
       <c r="D308" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -6332,7 +6338,7 @@
         <v>0.4</v>
       </c>
       <c r="D309" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -6346,7 +6352,7 @@
         <v>0.4</v>
       </c>
       <c r="D310" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -6360,7 +6366,7 @@
         <v>0.41</v>
       </c>
       <c r="D311" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -6374,7 +6380,7 @@
         <v>0.47</v>
       </c>
       <c r="D312" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -6388,7 +6394,7 @@
         <v>0.39</v>
       </c>
       <c r="D313" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -6402,7 +6408,7 @@
         <v>0.4</v>
       </c>
       <c r="D314" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -6416,7 +6422,7 @@
         <v>0.4</v>
       </c>
       <c r="D315" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6430,7 +6436,7 @@
         <v>0.39</v>
       </c>
       <c r="D316" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -6444,7 +6450,7 @@
         <v>0.4</v>
       </c>
       <c r="D317" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -6458,7 +6464,7 @@
         <v>0.41</v>
       </c>
       <c r="D318" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -6472,7 +6478,7 @@
         <v>0.47</v>
       </c>
       <c r="D319" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -6486,7 +6492,7 @@
         <v>0.4</v>
       </c>
       <c r="D320" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -6500,7 +6506,7 @@
         <v>0.39</v>
       </c>
       <c r="D321" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -6514,7 +6520,7 @@
         <v>0.39</v>
       </c>
       <c r="D322" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -6528,7 +6534,7 @@
         <v>0.38</v>
       </c>
       <c r="D323" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -6542,7 +6548,7 @@
         <v>0.4</v>
       </c>
       <c r="D324" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -6556,7 +6562,7 @@
         <v>0.41</v>
       </c>
       <c r="D325" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -6570,7 +6576,7 @@
         <v>0.43</v>
       </c>
       <c r="D326" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -6584,7 +6590,7 @@
         <v>0.39</v>
       </c>
       <c r="D327" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -6598,7 +6604,7 @@
         <v>0.4</v>
       </c>
       <c r="D328" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6612,7 +6618,7 @@
         <v>0.39</v>
       </c>
       <c r="D329" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -6626,7 +6632,7 @@
         <v>0.39</v>
       </c>
       <c r="D330" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -6640,7 +6646,7 @@
         <v>0.38</v>
       </c>
       <c r="D331" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -6654,7 +6660,7 @@
         <v>0.43</v>
       </c>
       <c r="D332" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -6668,7 +6674,7 @@
         <v>0.47</v>
       </c>
       <c r="D333" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -6682,7 +6688,7 @@
         <v>0.39</v>
       </c>
       <c r="D334" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -6696,7 +6702,7 @@
         <v>0.37</v>
       </c>
       <c r="D335" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -6710,7 +6716,7 @@
         <v>0.37</v>
       </c>
       <c r="D336" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -6724,7 +6730,7 @@
         <v>0.39</v>
       </c>
       <c r="D337" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -6738,7 +6744,7 @@
         <v>0.39</v>
       </c>
       <c r="D338" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -6752,7 +6758,7 @@
         <v>0.43</v>
       </c>
       <c r="D339" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -6766,7 +6772,7 @@
         <v>0.47</v>
       </c>
       <c r="D340" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -6780,7 +6786,7 @@
         <v>0.46</v>
       </c>
       <c r="D341" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -6794,7 +6800,7 @@
         <v>0.41</v>
       </c>
       <c r="D342" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -6808,7 +6814,7 @@
         <v>0.4</v>
       </c>
       <c r="D343" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -6822,7 +6828,7 @@
         <v>0.39</v>
       </c>
       <c r="D344" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -6836,7 +6842,7 @@
         <v>0.38</v>
       </c>
       <c r="D345" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -6850,7 +6856,7 @@
         <v>0.42</v>
       </c>
       <c r="D346" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -6864,7 +6870,7 @@
         <v>0.48</v>
       </c>
       <c r="D347" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -6878,7 +6884,7 @@
         <v>0.39</v>
       </c>
       <c r="D348" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -6892,7 +6898,7 @@
         <v>0.4</v>
       </c>
       <c r="D349" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -6906,7 +6912,7 @@
         <v>0.48</v>
       </c>
       <c r="D350" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -6920,7 +6926,7 @@
         <v>0.4</v>
       </c>
       <c r="D351" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -6934,7 +6940,7 @@
         <v>0.39</v>
       </c>
       <c r="D352" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -6948,7 +6954,7 @@
         <v>0.43</v>
       </c>
       <c r="D353" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -6962,7 +6968,7 @@
         <v>0.49</v>
       </c>
       <c r="D354" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -6976,7 +6982,7 @@
         <v>0.38</v>
       </c>
       <c r="D355" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -6990,7 +6996,7 @@
         <v>0.42</v>
       </c>
       <c r="D356" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -7004,7 +7010,7 @@
         <v>0.43</v>
       </c>
       <c r="D357" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -7018,7 +7024,7 @@
         <v>0.43</v>
       </c>
       <c r="D358" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -7032,7 +7038,7 @@
         <v>0.43</v>
       </c>
       <c r="D359" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -7046,7 +7052,7 @@
         <v>0.47</v>
       </c>
       <c r="D360" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -7060,7 +7066,7 @@
         <v>0.53</v>
       </c>
       <c r="D361" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -7074,7 +7080,7 @@
         <v>0.42</v>
       </c>
       <c r="D362" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -7088,7 +7094,7 @@
         <v>0.42</v>
       </c>
       <c r="D363" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -7102,7 +7108,7 @@
         <v>0.42</v>
       </c>
       <c r="D364" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -7116,7 +7122,7 @@
         <v>0.42</v>
       </c>
       <c r="D365" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -7130,7 +7136,7 @@
         <v>0.41</v>
       </c>
       <c r="D366" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -7144,7 +7150,7 @@
         <v>0.45</v>
       </c>
       <c r="D367" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -7158,7 +7164,7 @@
         <v>0.51</v>
       </c>
       <c r="D368" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -7172,7 +7178,7 @@
         <v>0.42</v>
       </c>
       <c r="D369" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -7186,7 +7192,7 @@
         <v>0.43</v>
       </c>
       <c r="D370" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -7200,7 +7206,7 @@
         <v>0.42</v>
       </c>
       <c r="D371" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -7214,7 +7220,7 @@
         <v>0.42</v>
       </c>
       <c r="D372" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -7228,7 +7234,7 @@
         <v>0.42</v>
       </c>
       <c r="D373" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -7242,7 +7248,7 @@
         <v>0.45</v>
       </c>
       <c r="D374" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7256,7 +7262,7 @@
         <v>0.51</v>
       </c>
       <c r="D375" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7270,7 +7276,7 @@
         <v>0.42</v>
       </c>
       <c r="D376" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7284,7 +7290,7 @@
         <v>0.43</v>
       </c>
       <c r="D377" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7298,7 +7304,7 @@
         <v>0.42</v>
       </c>
       <c r="D378" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7312,7 +7318,7 @@
         <v>0.42</v>
       </c>
       <c r="D379" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7326,7 +7332,7 @@
         <v>0.41</v>
       </c>
       <c r="D380" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7340,7 +7346,7 @@
         <v>0.45</v>
       </c>
       <c r="D381" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -7354,7 +7360,7 @@
         <v>0.51</v>
       </c>
       <c r="D382" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -7368,7 +7374,7 @@
         <v>0.42</v>
       </c>
       <c r="D383" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -7382,7 +7388,7 @@
         <v>0.42</v>
       </c>
       <c r="D384" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -7396,7 +7402,7 @@
         <v>0.42</v>
       </c>
       <c r="D385" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -7410,7 +7416,7 @@
         <v>0.43</v>
       </c>
       <c r="D386" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -7424,7 +7430,7 @@
         <v>0.47</v>
       </c>
       <c r="D387" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -7438,7 +7444,7 @@
         <v>0.46</v>
       </c>
       <c r="D388" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -7452,7 +7458,7 @@
         <v>0.5</v>
       </c>
       <c r="D389" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -7466,7 +7472,7 @@
         <v>0.42</v>
       </c>
       <c r="D390" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -7480,7 +7486,7 @@
         <v>0.42</v>
       </c>
       <c r="D391" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="392" spans="1:4">
@@ -7494,7 +7500,7 @@
         <v>0.42</v>
       </c>
       <c r="D392" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -7508,7 +7514,7 @@
         <v>0.41</v>
       </c>
       <c r="D393" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -7522,7 +7528,7 @@
         <v>0.41</v>
       </c>
       <c r="D394" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -7536,7 +7542,7 @@
         <v>0.44</v>
       </c>
       <c r="D395" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -7550,7 +7556,7 @@
         <v>0.5</v>
       </c>
       <c r="D396" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -7564,7 +7570,7 @@
         <v>0.4</v>
       </c>
       <c r="D397" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -7578,7 +7584,7 @@
         <v>0.41</v>
       </c>
       <c r="D398" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="399" spans="1:4">
@@ -7592,7 +7598,7 @@
         <v>0.41</v>
       </c>
       <c r="D399" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -7606,7 +7612,7 @@
         <v>0.41</v>
       </c>
       <c r="D400" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="401" spans="1:4">
@@ -7620,7 +7626,7 @@
         <v>0.41</v>
       </c>
       <c r="D401" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="402" spans="1:4">
@@ -7634,7 +7640,7 @@
         <v>0.44</v>
       </c>
       <c r="D402" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -7648,7 +7654,7 @@
         <v>0.5</v>
       </c>
       <c r="D403" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -7662,7 +7668,7 @@
         <v>0.41</v>
       </c>
       <c r="D404" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -7676,7 +7682,7 @@
         <v>0.41</v>
       </c>
       <c r="D405" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -7690,7 +7696,7 @@
         <v>0.48</v>
       </c>
       <c r="D406" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -7704,7 +7710,7 @@
         <v>0.4</v>
       </c>
       <c r="D407" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -7718,7 +7724,7 @@
         <v>0.41</v>
       </c>
       <c r="D408" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -7732,7 +7738,7 @@
         <v>0.43</v>
       </c>
       <c r="D409" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -7746,7 +7752,7 @@
         <v>0.5</v>
       </c>
       <c r="D410" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="411" spans="1:4">
@@ -7760,7 +7766,7 @@
         <v>0.42</v>
       </c>
       <c r="D411" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -7774,7 +7780,7 @@
         <v>0.4</v>
       </c>
       <c r="D412" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="413" spans="1:4">
@@ -7788,7 +7794,7 @@
         <v>0.4</v>
       </c>
       <c r="D413" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -7802,7 +7808,7 @@
         <v>0.4</v>
       </c>
       <c r="D414" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -7816,7 +7822,7 @@
         <v>0.43</v>
       </c>
       <c r="D415" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -7830,7 +7836,7 @@
         <v>0.43</v>
       </c>
       <c r="D416" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -7844,7 +7850,7 @@
         <v>0.48</v>
       </c>
       <c r="D417" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -7858,7 +7864,7 @@
         <v>0.4</v>
       </c>
       <c r="D418" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -7872,7 +7878,7 @@
         <v>0.4</v>
       </c>
       <c r="D419" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="420" spans="1:4">
@@ -7886,7 +7892,7 @@
         <v>0.4</v>
       </c>
       <c r="D420" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="421" spans="1:4">
@@ -7900,7 +7906,7 @@
         <v>0.38</v>
       </c>
       <c r="D421" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -7914,7 +7920,7 @@
         <v>0.39</v>
       </c>
       <c r="D422" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -7928,7 +7934,7 @@
         <v>0.41</v>
       </c>
       <c r="D423" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -7942,7 +7948,7 @@
         <v>0.46</v>
       </c>
       <c r="D424" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -7956,7 +7962,7 @@
         <v>0.4</v>
       </c>
       <c r="D425" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="426" spans="1:4">
@@ -7970,7 +7976,7 @@
         <v>0.4</v>
       </c>
       <c r="D426" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -7984,7 +7990,7 @@
         <v>0.4</v>
       </c>
       <c r="D427" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -7998,7 +8004,7 @@
         <v>0.4</v>
       </c>
       <c r="D428" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="429" spans="1:4">
@@ -8012,7 +8018,7 @@
         <v>0.39</v>
       </c>
       <c r="D429" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -8026,7 +8032,7 @@
         <v>0.42</v>
       </c>
       <c r="D430" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -8040,7 +8046,7 @@
         <v>0.47</v>
       </c>
       <c r="D431" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -8054,7 +8060,7 @@
         <v>0.4</v>
       </c>
       <c r="D432" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="433" spans="1:4">
@@ -8068,7 +8074,7 @@
         <v>0.41</v>
       </c>
       <c r="D433" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -8082,7 +8088,7 @@
         <v>0.41</v>
       </c>
       <c r="D434" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="435" spans="1:4">
@@ -8096,7 +8102,7 @@
         <v>0.4</v>
       </c>
       <c r="D435" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="436" spans="1:4">
@@ -8110,7 +8116,7 @@
         <v>0.4</v>
       </c>
       <c r="D436" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="437" spans="1:4">
@@ -8124,7 +8130,7 @@
         <v>0.43</v>
       </c>
       <c r="D437" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -8138,7 +8144,7 @@
         <v>0.49</v>
       </c>
       <c r="D438" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -8152,7 +8158,7 @@
         <v>0.41</v>
       </c>
       <c r="D439" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="440" spans="1:4">
@@ -8166,7 +8172,7 @@
         <v>0.41</v>
       </c>
       <c r="D440" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -8180,7 +8186,7 @@
         <v>0.41</v>
       </c>
       <c r="D441" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -8194,7 +8200,7 @@
         <v>0.4</v>
       </c>
       <c r="D442" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -8208,7 +8214,7 @@
         <v>0.4</v>
       </c>
       <c r="D443" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="444" spans="1:4">
@@ -8222,7 +8228,7 @@
         <v>0.43</v>
       </c>
       <c r="D444" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="445" spans="1:4">
@@ -8236,7 +8242,7 @@
         <v>0.49</v>
       </c>
       <c r="D445" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -8250,7 +8256,7 @@
         <v>0.41</v>
       </c>
       <c r="D446" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="447" spans="1:4">
@@ -8264,7 +8270,7 @@
         <v>0.41</v>
       </c>
       <c r="D447" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -8278,7 +8284,7 @@
         <v>0.4</v>
       </c>
       <c r="D448" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="449" spans="1:4">
@@ -8292,7 +8298,7 @@
         <v>0.47</v>
       </c>
       <c r="D449" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -8306,7 +8312,7 @@
         <v>0.4</v>
       </c>
       <c r="D450" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="451" spans="1:4">
@@ -8320,7 +8326,7 @@
         <v>0.42</v>
       </c>
       <c r="D451" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="452" spans="1:4">
@@ -8334,7 +8340,7 @@
         <v>0.48</v>
       </c>
       <c r="D452" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="453" spans="1:4">
@@ -8348,7 +8354,7 @@
         <v>0.4</v>
       </c>
       <c r="D453" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="454" spans="1:4">
@@ -8362,7 +8368,7 @@
         <v>0.39</v>
       </c>
       <c r="D454" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="455" spans="1:4">
@@ -8376,7 +8382,7 @@
         <v>0.4</v>
       </c>
       <c r="D455" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="456" spans="1:4">
@@ -8390,7 +8396,7 @@
         <v>0.39</v>
       </c>
       <c r="D456" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="457" spans="1:4">
@@ -8404,7 +8410,7 @@
         <v>0.39</v>
       </c>
       <c r="D457" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="458" spans="1:4">
@@ -8418,7 +8424,7 @@
         <v>0.42</v>
       </c>
       <c r="D458" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="459" spans="1:4">
@@ -8432,7 +8438,7 @@
         <v>0.47</v>
       </c>
       <c r="D459" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="460" spans="1:4">
@@ -8446,7 +8452,7 @@
         <v>0.39</v>
       </c>
       <c r="D460" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -8460,7 +8466,7 @@
         <v>0.4</v>
       </c>
       <c r="D461" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="462" spans="1:4">
@@ -8474,7 +8480,7 @@
         <v>0.4</v>
       </c>
       <c r="D462" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -8488,7 +8494,7 @@
         <v>0.39</v>
       </c>
       <c r="D463" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="464" spans="1:4">
@@ -8502,7 +8508,7 @@
         <v>0.39</v>
       </c>
       <c r="D464" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="465" spans="1:4">
@@ -8516,7 +8522,7 @@
         <v>0.43</v>
       </c>
       <c r="D465" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -8530,7 +8536,7 @@
         <v>0.49</v>
       </c>
       <c r="D466" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="467" spans="1:4">
@@ -8544,7 +8550,7 @@
         <v>0.4</v>
       </c>
       <c r="D467" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -8558,7 +8564,7 @@
         <v>0.42</v>
       </c>
       <c r="D468" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -8572,7 +8578,7 @@
         <v>0.4</v>
       </c>
       <c r="D469" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -8586,7 +8592,7 @@
         <v>0.4</v>
       </c>
       <c r="D470" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -8600,7 +8606,7 @@
         <v>0.4</v>
       </c>
       <c r="D471" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -8614,7 +8620,7 @@
         <v>0.45</v>
       </c>
       <c r="D472" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="473" spans="1:4">
@@ -8628,7 +8634,7 @@
         <v>0.49</v>
       </c>
       <c r="D473" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -8642,7 +8648,7 @@
         <v>0.4</v>
       </c>
       <c r="D474" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="475" spans="1:4">
@@ -8656,7 +8662,7 @@
         <v>0.41</v>
       </c>
       <c r="D475" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="476" spans="1:4">
@@ -8670,7 +8676,7 @@
         <v>0.4</v>
       </c>
       <c r="D476" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -8684,7 +8690,7 @@
         <v>0.41</v>
       </c>
       <c r="D477" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="478" spans="1:4">
@@ -8698,7 +8704,7 @@
         <v>0.39</v>
       </c>
       <c r="D478" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -8712,7 +8718,7 @@
         <v>0.43</v>
       </c>
       <c r="D479" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -8726,7 +8732,7 @@
         <v>0.48</v>
       </c>
       <c r="D480" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="481" spans="1:4">
@@ -8740,7 +8746,7 @@
         <v>0.4</v>
       </c>
       <c r="D481" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -8754,7 +8760,7 @@
         <v>0.4</v>
       </c>
       <c r="D482" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="483" spans="1:4">
@@ -8768,7 +8774,7 @@
         <v>0.39</v>
       </c>
       <c r="D483" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="484" spans="1:4">
@@ -8782,7 +8788,7 @@
         <v>0.38</v>
       </c>
       <c r="D484" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="485" spans="1:4">
@@ -8796,7 +8802,7 @@
         <v>0.41</v>
       </c>
       <c r="D485" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -8810,7 +8816,7 @@
         <v>0.47</v>
       </c>
       <c r="D486" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="487" spans="1:4">
@@ -8824,7 +8830,7 @@
         <v>0.39</v>
       </c>
       <c r="D487" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -8838,7 +8844,7 @@
         <v>0.4</v>
       </c>
       <c r="D488" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -8852,7 +8858,7 @@
         <v>0.4</v>
       </c>
       <c r="D489" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -8866,7 +8872,7 @@
         <v>0.4</v>
       </c>
       <c r="D490" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -8880,7 +8886,7 @@
         <v>0.38</v>
       </c>
       <c r="D491" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -8894,7 +8900,7 @@
         <v>0.42</v>
       </c>
       <c r="D492" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="493" spans="1:4">
@@ -8908,7 +8914,7 @@
         <v>0.48</v>
       </c>
       <c r="D493" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -8922,7 +8928,7 @@
         <v>0.4</v>
       </c>
       <c r="D494" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -8936,7 +8942,7 @@
         <v>0.41</v>
       </c>
       <c r="D495" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="496" spans="1:4">
@@ -8950,7 +8956,7 @@
         <v>0.41</v>
       </c>
       <c r="D496" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -8964,7 +8970,7 @@
         <v>0.41</v>
       </c>
       <c r="D497" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -8978,7 +8984,7 @@
         <v>0.4</v>
       </c>
       <c r="D498" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -8992,7 +8998,7 @@
         <v>0.42</v>
       </c>
       <c r="D499" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -9006,7 +9012,7 @@
         <v>0.47</v>
       </c>
       <c r="D500" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -9020,7 +9026,7 @@
         <v>0.4</v>
       </c>
       <c r="D501" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="502" spans="1:4">
@@ -9034,7 +9040,7 @@
         <v>0.41</v>
       </c>
       <c r="D502" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -9048,7 +9054,7 @@
         <v>0.42</v>
       </c>
       <c r="D503" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -9062,7 +9068,7 @@
         <v>0.41</v>
       </c>
       <c r="D504" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="505" spans="1:4">
@@ -9076,7 +9082,7 @@
         <v>0.43</v>
       </c>
       <c r="D505" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="506" spans="1:4">
@@ -9090,7 +9096,7 @@
         <v>0.43</v>
       </c>
       <c r="D506" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="507" spans="1:4">
@@ -9104,7 +9110,7 @@
         <v>0.47</v>
       </c>
       <c r="D507" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -9118,7 +9124,7 @@
         <v>0.39</v>
       </c>
       <c r="D508" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="509" spans="1:4">
@@ -9132,7 +9138,7 @@
         <v>0.4</v>
       </c>
       <c r="D509" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="510" spans="1:4">
@@ -9146,7 +9152,7 @@
         <v>0.41</v>
       </c>
       <c r="D510" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="511" spans="1:4">
@@ -9160,7 +9166,7 @@
         <v>0.4</v>
       </c>
       <c r="D511" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="512" spans="1:4">
@@ -9174,7 +9180,7 @@
         <v>0.39</v>
       </c>
       <c r="D512" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="513" spans="1:4">
@@ -9188,7 +9194,7 @@
         <v>0.41</v>
       </c>
       <c r="D513" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="514" spans="1:4">
@@ -9202,7 +9208,7 @@
         <v>0.46</v>
       </c>
       <c r="D514" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="515" spans="1:4">
@@ -9216,7 +9222,7 @@
         <v>0.39</v>
       </c>
       <c r="D515" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="516" spans="1:4">
@@ -9230,7 +9236,7 @@
         <v>0.4</v>
       </c>
       <c r="D516" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="517" spans="1:4">
@@ -9244,7 +9250,7 @@
         <v>0.39</v>
       </c>
       <c r="D517" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="518" spans="1:4">
@@ -9258,7 +9264,7 @@
         <v>0.4</v>
       </c>
       <c r="D518" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="519" spans="1:4">
@@ -9272,7 +9278,7 @@
         <v>0.39</v>
       </c>
       <c r="D519" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -9286,7 +9292,7 @@
         <v>0.41</v>
       </c>
       <c r="D520" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="521" spans="1:4">
@@ -9300,7 +9306,7 @@
         <v>0.46</v>
       </c>
       <c r="D521" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="522" spans="1:4">
@@ -9314,7 +9320,7 @@
         <v>0.37</v>
       </c>
       <c r="D522" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="523" spans="1:4">
@@ -9328,7 +9334,7 @@
         <v>0.39</v>
       </c>
       <c r="D523" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="524" spans="1:4">
@@ -9342,7 +9348,7 @@
         <v>0.39</v>
       </c>
       <c r="D524" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="525" spans="1:4">
@@ -9356,7 +9362,7 @@
         <v>0.39</v>
       </c>
       <c r="D525" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="526" spans="1:4">
@@ -9370,7 +9376,7 @@
         <v>0.38</v>
       </c>
       <c r="D526" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="527" spans="1:4">
@@ -9384,7 +9390,7 @@
         <v>0.41</v>
       </c>
       <c r="D527" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="528" spans="1:4">
@@ -9398,7 +9404,7 @@
         <v>0.46</v>
       </c>
       <c r="D528" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="529" spans="1:4">
@@ -9412,7 +9418,7 @@
         <v>0.38</v>
       </c>
       <c r="D529" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="530" spans="1:4">
@@ -9426,7 +9432,7 @@
         <v>0.4</v>
       </c>
       <c r="D530" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="531" spans="1:4">
@@ -9440,7 +9446,7 @@
         <v>0.4</v>
       </c>
       <c r="D531" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="532" spans="1:4">
@@ -9454,7 +9460,7 @@
         <v>0.37</v>
       </c>
       <c r="D532" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="533" spans="1:4">
@@ -9468,7 +9474,7 @@
         <v>0.37</v>
       </c>
       <c r="D533" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="534" spans="1:4">
@@ -9482,7 +9488,35 @@
         <v>0.42</v>
       </c>
       <c r="D534" t="s">
-        <v>541</v>
+        <v>543</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4">
+      <c r="A535" t="s">
+        <v>537</v>
+      </c>
+      <c r="B535">
+        <v>0.46</v>
+      </c>
+      <c r="C535">
+        <v>0.48</v>
+      </c>
+      <c r="D535" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4">
+      <c r="A536" t="s">
+        <v>538</v>
+      </c>
+      <c r="B536">
+        <v>0.39</v>
+      </c>
+      <c r="C536">
+        <v>0.4</v>
+      </c>
+      <c r="D536" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>